<commit_message>
Added Git Ignore File
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singhnitinkum.vinod\Desktop\excel-diff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6343E172-51E5-4D65-BBA3-FE137A4129F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAEB3D9-F9CA-4939-8A64-C94393932201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{63FB5C2F-3322-4A33-AE12-BF37764062A0}"/>
   </bookViews>
@@ -35,10 +35,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>SR.No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Nitin Singh</t>
+  </si>
+  <si>
+    <t>Pravin Shukla</t>
+  </si>
+  <si>
+    <t>Maddy Singh</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,14 +431,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A91562-AB95-45AD-B2A1-1D64ED08C75C}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Husky to ignore
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singhnitinkum.vinod\Desktop\excel-diff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAEB3D9-F9CA-4939-8A64-C94393932201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AB41E4-234A-473D-BDB5-8E563D3ADB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{63FB5C2F-3322-4A33-AE12-BF37764062A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SR.No</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Maddy Singh</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A91562-AB95-45AD-B2A1-1D64ED08C75C}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,6 +474,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Again Done some modification
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\singhnitinkum.vinod\Desktop\excel-diff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9807569-436B-4377-9EC4-506BBEB92860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309128B6-D3CB-463D-B523-7637C02CC62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" xr2:uid="{63FB5C2F-3322-4A33-AE12-BF37764062A0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>SR.No</t>
   </si>
@@ -84,25 +84,22 @@
     <t>Soni</t>
   </si>
   <si>
-    <t xml:space="preserve">Maddy </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mahesh </t>
   </si>
   <si>
     <t>Dhiraj</t>
   </si>
   <si>
-    <t>Piyush  Kumar</t>
-  </si>
-  <si>
-    <t>Dharam Kumar</t>
-  </si>
-  <si>
     <t>Bitu Kumar</t>
   </si>
   <si>
     <t xml:space="preserve">Pravin Kumar </t>
+  </si>
+  <si>
+    <t>Dharam Kumar New</t>
+  </si>
+  <si>
+    <t>Piyush  Kumar  New</t>
   </si>
 </sst>
 </file>
@@ -485,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A91562-AB95-45AD-B2A1-1D64ED08C75C}">
   <dimension ref="A2:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -542,9 +539,6 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -557,10 +551,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -571,7 +565,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -596,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>

</xml_diff>